<commit_message>
Actualizar (GAd2-EeA) y eliminar apoyos del curso anterior
</commit_message>
<xml_diff>
--- a/.controlPGAFP.xlsx
+++ b/.controlPGAFP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\gitHub\PGA_FP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084E30E9-E89C-4C93-8458-EC6D8B0D43D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3FBEBB-E742-440B-87CC-486873ED7C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8928" yWindow="12" windowWidth="14100" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="30">
   <si>
     <t>RA1</t>
   </si>
@@ -103,16 +103,35 @@
   </si>
   <si>
     <t>Trab. Inves colec</t>
+  </si>
+  <si>
+    <t>Trab inv colect</t>
+  </si>
+  <si>
+    <t>Act intercon postinvestig</t>
+  </si>
+  <si>
+    <t>Elaboración de la documentación</t>
+  </si>
+  <si>
+    <t>????</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,8 +157,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L91"/>
+  <dimension ref="B2:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="M68" sqref="M68"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,12 +694,6 @@
       <c r="F19">
         <v>100</v>
       </c>
-      <c r="G19">
-        <v>70</v>
-      </c>
-      <c r="J19">
-        <v>30</v>
-      </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
@@ -691,7 +705,7 @@
       <c r="F20">
         <v>30</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>70</v>
       </c>
     </row>
@@ -702,10 +716,13 @@
       <c r="E21">
         <v>10</v>
       </c>
+      <c r="G21" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J21">
         <v>50</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="1">
         <v>50</v>
       </c>
     </row>
@@ -932,7 +949,7 @@
       <c r="E42">
         <v>10</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>100</v>
       </c>
     </row>
@@ -943,7 +960,7 @@
       <c r="E43">
         <v>10</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="1">
         <v>100</v>
       </c>
     </row>
@@ -1215,7 +1232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
         <v>17</v>
       </c>
@@ -1223,7 +1240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>5</v>
       </c>
@@ -1249,79 +1266,112 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>7</v>
       </c>
       <c r="E68">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F68">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
         <v>8</v>
       </c>
       <c r="E69">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F69">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
         <v>9</v>
       </c>
       <c r="E70">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K70">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D71" t="s">
         <v>10</v>
       </c>
       <c r="E71">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <v>50</v>
+      </c>
+      <c r="K71">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D72" t="s">
         <v>11</v>
       </c>
       <c r="E72">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <v>50</v>
+      </c>
+      <c r="K72">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
         <v>12</v>
       </c>
       <c r="E73">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
         <v>13</v>
       </c>
       <c r="E74">
         <v>10</v>
       </c>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
         <v>14</v>
       </c>
       <c r="E75" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D76" t="s">
         <v>15</v>
       </c>
       <c r="E76" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D77" t="s">
         <v>16</v>
       </c>
@@ -1329,7 +1379,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D78" t="s">
         <v>17</v>
       </c>
@@ -1337,7 +1387,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>6</v>
       </c>
@@ -1362,91 +1412,145 @@
       <c r="K80" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="L80" t="s">
+        <v>26</v>
+      </c>
+      <c r="M80" t="s">
+        <v>27</v>
+      </c>
+      <c r="O80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
         <v>7</v>
       </c>
       <c r="E81">
         <v>10</v>
       </c>
-      <c r="F81">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="K81">
+        <v>50</v>
+      </c>
+      <c r="L81">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
         <v>8</v>
       </c>
       <c r="E82">
         <v>10</v>
       </c>
-    </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="K82">
+        <v>50</v>
+      </c>
+      <c r="M82">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D83" t="s">
         <v>9</v>
       </c>
       <c r="E83">
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="K83">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D84" t="s">
         <v>10</v>
       </c>
       <c r="E84">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="K84">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
         <v>11</v>
       </c>
       <c r="E85">
         <v>10</v>
       </c>
-    </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="K85">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
         <v>12</v>
       </c>
       <c r="E86">
         <v>10</v>
       </c>
-    </row>
-    <row r="87" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="G86">
+        <v>50</v>
+      </c>
+      <c r="K86">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
         <v>13</v>
       </c>
       <c r="E87">
         <v>10</v>
       </c>
-    </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="G87">
+        <v>50</v>
+      </c>
+      <c r="K87">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D88" t="s">
         <v>14</v>
       </c>
       <c r="E88">
         <v>10</v>
       </c>
-    </row>
-    <row r="89" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="G88">
+        <v>50</v>
+      </c>
+      <c r="K88">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
         <v>15</v>
       </c>
       <c r="E89">
         <v>10</v>
       </c>
-    </row>
-    <row r="90" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="K89">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D90" t="s">
         <v>16</v>
       </c>
       <c r="E90">
         <v>10</v>
       </c>
-    </row>
-    <row r="91" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="K90">
+        <v>50</v>
+      </c>
+      <c r="O90">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="91" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
         <v>17</v>
       </c>

</xml_diff>